<commit_message>
hw + blok schema
</commit_message>
<xml_diff>
--- a/hw/ESP32 Pins (copy 2).xlsx
+++ b/hw/ESP32 Pins (copy 2).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="334">
   <si>
     <t>No.</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>HIGH</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>TXD0</t>
@@ -557,6 +560,9 @@
   </si>
   <si>
     <t>EMAC_RXD0</t>
+  </si>
+  <si>
+    <t>LED_STRIP</t>
   </si>
   <si>
     <t>IO26</t>
@@ -1745,7 +1751,9 @@
       <c r="T2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U2" s="2"/>
+      <c r="U2" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
@@ -1758,13 +1766,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>23</v>
@@ -1777,18 +1785,20 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="U3" t="s">
+        <v>33</v>
+      </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
@@ -1801,49 +1811,51 @@
         <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U4" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
@@ -1856,13 +1868,13 @@
         <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>23</v>
@@ -1875,7 +1887,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1884,7 +1896,9 @@
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
+      <c r="U5" t="s">
+        <v>46</v>
+      </c>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
@@ -1897,41 +1911,41 @@
         <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
@@ -1948,13 +1962,13 @@
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1963,26 +1977,28 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U7" s="2"/>
+      <c r="U7" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
@@ -1995,19 +2011,19 @@
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -2016,22 +2032,24 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q8" s="3"/>
       <c r="R8" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
+      <c r="U8" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
@@ -2044,19 +2062,19 @@
         <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -2065,22 +2083,24 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Q9" s="3"/>
       <c r="R9" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
+      <c r="U9" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
@@ -2093,19 +2113,19 @@
         <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -2114,22 +2134,24 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="Q10" s="3"/>
       <c r="R10" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
+      <c r="U10" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
@@ -2142,19 +2164,19 @@
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2163,22 +2185,24 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Q11" s="3"/>
       <c r="R11" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
+      <c r="U11" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
@@ -2191,19 +2215,19 @@
         <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -2212,22 +2236,24 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Q12" s="3"/>
       <c r="R12" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
+      <c r="U12" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
@@ -2240,19 +2266,19 @@
         <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -2261,20 +2287,22 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
+      <c r="U13" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
@@ -2287,53 +2315,55 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U14" t="s">
         <v>104</v>
       </c>
-      <c r="R14" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="S14" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
@@ -2346,47 +2376,49 @@
         <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
+      <c r="U15" t="s">
+        <v>114</v>
+      </c>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
@@ -2399,47 +2431,49 @@
         <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
+      <c r="U16" t="s">
+        <v>123</v>
+      </c>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
@@ -2452,51 +2486,53 @@
         <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="P17" s="2"/>
       <c r="Q17" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="T17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U17" s="2"/>
+      <c r="U17" t="s">
+        <v>132</v>
+      </c>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
@@ -2509,16 +2545,16 @@
         <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -2528,23 +2564,23 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T18" s="2"/>
       <c r="U18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
@@ -2558,16 +2594,16 @@
         <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -2577,23 +2613,23 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T19" s="2"/>
       <c r="U19" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
@@ -2607,13 +2643,13 @@
         <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2622,18 +2658,18 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
@@ -2650,13 +2686,13 @@
         <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -2665,19 +2701,19 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
@@ -2695,13 +2731,13 @@
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -2709,23 +2745,25 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
+      <c r="U22" t="s">
+        <v>160</v>
+      </c>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
@@ -2738,13 +2776,13 @@
         <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -2752,25 +2790,27 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
+      <c r="U23" t="s">
+        <v>165</v>
+      </c>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
@@ -2783,13 +2823,13 @@
         <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -2798,18 +2838,18 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
@@ -2826,24 +2866,24 @@
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -2853,12 +2893,14 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
+      <c r="U25" s="4" t="s">
+        <v>180</v>
+      </c>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
@@ -2871,24 +2913,24 @@
         <v>11</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -2898,13 +2940,13 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
-      <c r="U26" s="4" t="s">
-        <v>185</v>
+      <c r="U26" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
@@ -2918,23 +2960,23 @@
         <v>12</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -2945,13 +2987,13 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
-      <c r="U27" s="4" t="s">
-        <v>192</v>
+      <c r="U27" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
@@ -2965,23 +3007,23 @@
         <v>8</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -2994,7 +3036,7 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
@@ -3010,23 +3052,23 @@
         <v>9</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -3039,7 +3081,7 @@
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
@@ -3055,22 +3097,22 @@
         <v>6</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -3084,10 +3126,12 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="S30" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="T30" s="2"/>
-      <c r="U30" s="2"/>
+      <c r="U30" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
@@ -3100,22 +3144,22 @@
         <v>7</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -3129,10 +3173,12 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
+      <c r="U31" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
       <c r="X31" s="2"/>
@@ -3145,22 +3191,22 @@
         <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -3174,10 +3220,12 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
       <c r="S32" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
+      <c r="U32" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
       <c r="X32" s="2"/>
@@ -3190,22 +3238,22 @@
         <v>5</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -3219,10 +3267,12 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
+      <c r="U33" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
       <c r="X33" s="2"/>
@@ -31314,47 +31364,47 @@
         <v>2</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B2" s="7">
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B3" s="7">
         <v>2</v>
@@ -31363,366 +31413,366 @@
         <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>227</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B4" s="7">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B5" s="7">
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B6" s="7">
         <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B7" s="7">
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B8" s="7">
         <v>7</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B9" s="7">
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B10" s="7">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B11" s="7">
         <v>10</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B12" s="7">
         <v>11</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B13" s="7">
         <v>12</v>
@@ -31731,36 +31781,36 @@
         <v>21</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B14" s="7">
         <v>13</v>
@@ -31769,36 +31819,36 @@
         <v>21</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B15" s="7">
         <v>14</v>
@@ -31807,36 +31857,36 @@
         <v>21</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B16" s="7">
         <v>15</v>
@@ -31845,36 +31895,36 @@
         <v>21</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B17" s="7">
         <v>16</v>
@@ -31883,36 +31933,36 @@
         <v>21</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F17" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>188</v>
-      </c>
       <c r="H17" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B18" s="7">
         <v>17</v>
@@ -31921,36 +31971,36 @@
         <v>21</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H18" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="J18" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J18" s="7" t="s">
-        <v>120</v>
-      </c>
       <c r="K18" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B19" s="7">
         <v>18</v>
@@ -31959,71 +32009,71 @@
         <v>21</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H19" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="J19" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="J19" s="7" t="s">
-        <v>101</v>
-      </c>
       <c r="K19" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B20" s="7">
         <v>19</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B21" s="7">
         <v>20</v>
@@ -32032,36 +32082,36 @@
         <v>21</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H21" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="I21" s="7" t="s">
+      <c r="J21" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="J21" s="7" t="s">
-        <v>111</v>
-      </c>
       <c r="K21" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B22" s="7">
         <v>21</v>
@@ -32070,36 +32120,36 @@
         <v>21</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H22" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I22" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="J22" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="J22" s="7" t="s">
-        <v>129</v>
-      </c>
       <c r="K22" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="7" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B23" s="7">
         <v>22</v>
@@ -32108,36 +32158,36 @@
         <v>21</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H23" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="J23" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B24" s="7">
         <v>23</v>
@@ -32146,10 +32196,10 @@
         <v>21</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>26</v>
@@ -32158,24 +32208,24 @@
         <v>24</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B25" s="7">
         <v>24</v>
@@ -32184,36 +32234,36 @@
         <v>21</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="E25" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="H25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I25" s="7" t="s">
-        <v>51</v>
-      </c>
       <c r="J25" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B26" s="7">
         <v>25</v>
@@ -32222,71 +32272,71 @@
         <v>21</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="7" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B27" s="7">
         <v>26</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B28" s="7">
         <v>27</v>
@@ -32295,36 +32345,36 @@
         <v>21</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B29" s="3">
         <v>28</v>
@@ -32333,36 +32383,36 @@
         <v>21</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E29" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="G29" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B30" s="3">
         <v>29</v>
@@ -32371,36 +32421,36 @@
         <v>21</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="G30" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B31" s="3">
         <v>30</v>
@@ -32409,36 +32459,36 @@
         <v>21</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B32" s="3">
         <v>31</v>
@@ -32447,36 +32497,36 @@
         <v>21</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="G32" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B33" s="3">
         <v>32</v>
@@ -32485,36 +32535,36 @@
         <v>21</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="E33" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="G33" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B34" s="3">
         <v>33</v>
@@ -32523,36 +32573,36 @@
         <v>21</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="G34" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="7" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B35" s="7">
         <v>34</v>
@@ -32561,36 +32611,36 @@
         <v>21</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B36" s="7">
         <v>35</v>
@@ -32599,36 +32649,36 @@
         <v>21</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B37" s="7">
         <v>36</v>
@@ -32637,71 +32687,71 @@
         <v>21</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="7" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B38" s="7">
         <v>37</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B39" s="7">
         <v>38</v>
@@ -32710,36 +32760,36 @@
         <v>21</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E39" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F39" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="F39" s="7" t="s">
-        <v>154</v>
-      </c>
       <c r="G39" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B40" s="7">
         <v>39</v>
@@ -32748,36 +32798,36 @@
         <v>21</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E40" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F40" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="F40" s="7" t="s">
-        <v>165</v>
-      </c>
       <c r="G40" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B41" s="7">
         <v>40</v>
@@ -32786,36 +32836,36 @@
         <v>21</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B42" s="7">
         <v>41</v>
@@ -32824,36 +32874,36 @@
         <v>21</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B43" s="7">
         <v>42</v>
@@ -32862,456 +32912,456 @@
         <v>21</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="7" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B44" s="7">
         <v>43</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="7" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B45" s="7">
         <v>44</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K45" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="7" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B46" s="7">
         <v>45</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="7" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B47" s="7">
         <v>46</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K47" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="7" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B48" s="7">
         <v>47</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="7" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B49" s="7">
         <v>48</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K49" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="7" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B50" s="7">
         <v>49</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K50" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="L51" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="L52" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="L53" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="L54" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="L55" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="L56" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="L57" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="L58" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="L59" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="L60" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="L61" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="L62" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="L63" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="L64" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="L65" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="L66" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="L67" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="L68" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="L69" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="L70" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="L71" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="L72" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="L73" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="L74" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="L75" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="L76" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="L77" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="L78" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="L79" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="L80" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="L81" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="L82" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="L83" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="L84" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="L85" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="L86" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
hw - changed uart2 pins, latex- ridici jednotka
</commit_message>
<xml_diff>
--- a/hw/ESP32 Pins (copy 2).xlsx
+++ b/hw/ESP32 Pins (copy 2).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="335">
   <si>
     <t>No.</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>EMAC_TX_ER</t>
+  </si>
+  <si>
+    <t>U2RXD</t>
   </si>
   <si>
     <t>IO05</t>
@@ -436,9 +439,6 @@
     <t xml:space="preserve">Not available on WROVER</t>
   </si>
   <si>
-    <t>U2RXD</t>
-  </si>
-  <si>
     <t>EMAC_CLK_OUT</t>
   </si>
   <si>
@@ -476,6 +476,9 @@
   </si>
   <si>
     <t>HS1_DATA7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pull up</t>
   </si>
   <si>
     <t>IO19</t>
@@ -1949,7 +1952,9 @@
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
+      <c r="U6" t="s">
+        <v>55</v>
+      </c>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
@@ -1962,13 +1967,13 @@
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1977,20 +1982,20 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="2" t="s">
@@ -2011,19 +2016,19 @@
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -2032,18 +2037,18 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q8" s="3"/>
       <c r="R8" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
@@ -2062,19 +2067,19 @@
         <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -2083,18 +2088,18 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q9" s="3"/>
       <c r="R9" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
@@ -2113,19 +2118,19 @@
         <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -2134,18 +2139,18 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q10" s="3"/>
       <c r="R10" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
@@ -2164,19 +2169,19 @@
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2185,18 +2190,18 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="Q11" s="3"/>
       <c r="R11" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
@@ -2215,19 +2220,19 @@
         <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -2236,18 +2241,18 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="Q12" s="3"/>
       <c r="R12" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
@@ -2266,19 +2271,19 @@
         <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -2287,16 +2292,16 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
@@ -2315,54 +2320,54 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="T14" s="2" t="s">
         <v>43</v>
       </c>
       <c r="U14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -2376,48 +2381,48 @@
         <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
@@ -2431,48 +2436,48 @@
         <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
       <c r="U16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
@@ -2486,52 +2491,52 @@
         <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="P17" s="2"/>
       <c r="Q17" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="T17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="U17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
@@ -2545,16 +2550,16 @@
         <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -2564,7 +2569,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2" t="s">
-        <v>138</v>
+        <v>55</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -2579,9 +2584,6 @@
         <v>141</v>
       </c>
       <c r="T18" s="2"/>
-      <c r="U18" t="s">
-        <v>138</v>
-      </c>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
@@ -2603,7 +2605,7 @@
         <v>143</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -2673,7 +2675,9 @@
       </c>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
+      <c r="U20" s="4" t="s">
+        <v>152</v>
+      </c>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
@@ -2686,13 +2690,13 @@
         <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -2701,19 +2705,19 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
@@ -2731,13 +2735,13 @@
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -2745,24 +2749,24 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
@@ -2776,13 +2780,13 @@
         <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -2790,26 +2794,26 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
@@ -2823,13 +2827,13 @@
         <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -2838,18 +2842,18 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
@@ -2866,24 +2870,24 @@
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -2893,13 +2897,13 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
-      <c r="U25" s="4" t="s">
-        <v>180</v>
+      <c r="U25" s="2" t="s">
+        <v>181</v>
       </c>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
@@ -2913,24 +2917,24 @@
         <v>11</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -2940,13 +2944,13 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
@@ -2960,23 +2964,23 @@
         <v>12</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -2987,13 +2991,13 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
@@ -3007,23 +3011,23 @@
         <v>8</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -3036,7 +3040,7 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
@@ -3052,23 +3056,23 @@
         <v>9</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -3081,7 +3085,7 @@
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
@@ -3097,22 +3101,22 @@
         <v>6</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -3126,7 +3130,7 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="S30" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="T30" s="2"/>
       <c r="U30" s="2" t="s">
@@ -3144,22 +3148,22 @@
         <v>7</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -3173,7 +3177,7 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="T31" s="2"/>
       <c r="U31" s="2" t="s">
@@ -3191,22 +3195,22 @@
         <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -3220,7 +3224,7 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
       <c r="S32" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="T32" s="2"/>
       <c r="U32" s="2" t="s">
@@ -3238,22 +3242,22 @@
         <v>5</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -3267,7 +3271,7 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="T33" s="2"/>
       <c r="U33" s="2" t="s">
@@ -31364,47 +31368,47 @@
         <v>2</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B2" s="7">
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B3" s="7">
         <v>2</v>
@@ -31413,366 +31417,366 @@
         <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B4" s="7">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B5" s="7">
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B6" s="7">
         <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B7" s="7">
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B8" s="7">
         <v>7</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B9" s="7">
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B10" s="7">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B11" s="7">
         <v>10</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B12" s="7">
         <v>11</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B13" s="7">
         <v>12</v>
@@ -31781,36 +31785,36 @@
         <v>21</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B14" s="7">
         <v>13</v>
@@ -31819,36 +31823,36 @@
         <v>21</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B15" s="7">
         <v>14</v>
@@ -31857,36 +31861,36 @@
         <v>21</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B16" s="7">
         <v>15</v>
@@ -31895,36 +31899,36 @@
         <v>21</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B17" s="7">
         <v>16</v>
@@ -31933,36 +31937,36 @@
         <v>21</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B18" s="7">
         <v>17</v>
@@ -31971,36 +31975,36 @@
         <v>21</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H18" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="J18" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="J18" s="7" t="s">
-        <v>121</v>
-      </c>
       <c r="K18" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B19" s="7">
         <v>18</v>
@@ -32009,71 +32013,71 @@
         <v>21</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H19" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="J19" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="J19" s="7" t="s">
-        <v>102</v>
-      </c>
       <c r="K19" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B20" s="7">
         <v>19</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B21" s="7">
         <v>20</v>
@@ -32082,36 +32086,36 @@
         <v>21</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H21" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I21" s="7" t="s">
+      <c r="J21" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="J21" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="K21" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B22" s="7">
         <v>21</v>
@@ -32120,36 +32124,36 @@
         <v>21</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H22" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I22" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="J22" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="J22" s="7" t="s">
-        <v>130</v>
-      </c>
       <c r="K22" s="7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B23" s="7">
         <v>22</v>
@@ -32158,10 +32162,10 @@
         <v>21</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>39</v>
@@ -32176,18 +32180,18 @@
         <v>40</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B24" s="7">
         <v>23</v>
@@ -32196,10 +32200,10 @@
         <v>21</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>26</v>
@@ -32208,24 +32212,24 @@
         <v>24</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B25" s="7">
         <v>24</v>
@@ -32234,7 +32238,7 @@
         <v>21</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>50</v>
@@ -32252,18 +32256,18 @@
         <v>52</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B26" s="7">
         <v>25</v>
@@ -32272,66 +32276,66 @@
         <v>21</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>140</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>138</v>
+        <v>55</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B27" s="7">
         <v>26</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -32354,27 +32358,27 @@
         <v>144</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B29" s="3">
         <v>28</v>
@@ -32383,36 +32387,36 @@
         <v>21</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="G29" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B30" s="3">
         <v>29</v>
@@ -32421,36 +32425,36 @@
         <v>21</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="G30" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B31" s="3">
         <v>30</v>
@@ -32459,36 +32463,36 @@
         <v>21</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B32" s="3">
         <v>31</v>
@@ -32497,36 +32501,36 @@
         <v>21</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="G32" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B33" s="3">
         <v>32</v>
@@ -32535,36 +32539,36 @@
         <v>21</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E33" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="G33" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B34" s="3">
         <v>33</v>
@@ -32573,36 +32577,36 @@
         <v>21</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E34" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="G34" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B35" s="7">
         <v>34</v>
@@ -32611,31 +32615,31 @@
         <v>21</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
@@ -32655,30 +32659,30 @@
         <v>150</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B37" s="7">
         <v>36</v>
@@ -32687,71 +32691,71 @@
         <v>21</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B38" s="7">
         <v>37</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B39" s="7">
         <v>38</v>
@@ -32760,36 +32764,36 @@
         <v>21</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E39" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F39" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="F39" s="7" t="s">
-        <v>155</v>
-      </c>
       <c r="G39" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B40" s="7">
         <v>39</v>
@@ -32798,31 +32802,31 @@
         <v>21</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E40" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F40" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="F40" s="7" t="s">
-        <v>166</v>
-      </c>
       <c r="G40" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
@@ -32836,31 +32840,31 @@
         <v>21</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>46</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
@@ -32874,36 +32878,36 @@
         <v>21</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B43" s="7">
         <v>42</v>
@@ -32912,456 +32916,456 @@
         <v>21</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B44" s="7">
         <v>43</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B45" s="7">
         <v>44</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K45" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="7" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B46" s="7">
         <v>45</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B47" s="7">
         <v>46</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K47" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B48" s="7">
         <v>47</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B49" s="7">
         <v>48</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K49" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B50" s="7">
         <v>49</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K50" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="L51" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="L52" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="L53" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="L54" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="L55" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="L56" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="L57" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="L58" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="L59" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="L60" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="L61" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="L62" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="L63" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="L64" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="L65" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="L66" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="L67" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="L68" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="L69" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="L70" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="L71" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="L72" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="L73" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="L74" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="L75" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="L76" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="L77" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="L78" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="L79" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="L80" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="L81" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="L82" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="L83" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="L84" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="L85" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="L86" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1"/>

</xml_diff>